<commit_message>
switched back to realistic annual vehicle mileages
</commit_message>
<xml_diff>
--- a/analysis dimensions.xlsx
+++ b/analysis dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steff\Documents\Studium - UW\PUBPOL 594 A - Economic Approaches To Environmental Management\Project\tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8662718C-1713-4CEA-8697-6CF49FA1532F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC4277D-FBE9-4681-8E5B-66EB2A7750C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-165" yWindow="-16365" windowWidth="29130" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -118,7 +118,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -403,7 +402,7 @@
   <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,42 +417,42 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
-        <v>2</v>
+      <c r="B6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>6</v>
       </c>
     </row>
@@ -463,7 +462,7 @@
       </c>
       <c r="B8" s="3">
         <f>PRODUCT(B3:B7)</f>
-        <v>1728</v>
+        <v>2592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>